<commit_message>
nhập writing và speaking
</commit_message>
<xml_diff>
--- a/speaking-test.xlsx
+++ b/speaking-test.xlsx
@@ -3,7 +3,10 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Topics" sheetId="1" r:id="rId1"/>
+    <sheet name="Exams" sheetId="1" r:id="rId1"/>
+    <sheet name="Parts" sheetId="2" r:id="rId2"/>
+    <sheet name="Questions" sheetId="3" r:id="rId3"/>
+    <sheet name="Answers" sheetId="4" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
@@ -397,98 +400,420 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Topic</v>
+        <v>title</v>
       </c>
       <c r="B1" t="str">
-        <v>Vietnamese</v>
+        <v>description</v>
       </c>
       <c r="C1" t="str">
-        <v>Level</v>
+        <v>difficulty</v>
       </c>
       <c r="D1" t="str">
-        <v>Time</v>
+        <v>estimated_time</v>
+      </c>
+      <c r="E1" t="str">
+        <v>exam_type</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Describe your hometown and what makes it special.</v>
+        <v>Speaking Test - Assessment</v>
       </c>
       <c r="B2" t="str">
-        <v>Mô tả quê hương của bạn và điều gì làm nó đặc biệt.</v>
+        <v>Đề thi Speaking - 11 câu hỏi theo chuẩn đánh giá năng lực nói</v>
       </c>
       <c r="C2" t="str">
-        <v>Medium</v>
-      </c>
-      <c r="D2" t="str">
-        <v>2-3 minutes</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Talk about a book that has influenced your life.</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Nói về một cuốn sách đã ảnh hưởng đến cuộc sống của bạn.</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Medium</v>
-      </c>
-      <c r="D3" t="str">
-        <v>2-3 minutes</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Discuss the importance of learning English in today's world.</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Thảo luận về tầm quan trọng của việc học tiếng Anh trong thế giới ngày nay.</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Medium</v>
-      </c>
-      <c r="D4" t="str">
-        <v>2-3 minutes</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Describe your favorite place to relax and why you enjoy it.</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Mô tả nơi yêu thích để thư giãn và lý do bạn thích nó.</v>
-      </c>
-      <c r="C5" t="str">
-        <v>Easy</v>
-      </c>
-      <c r="D5" t="str">
-        <v>2-3 minutes</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Talk about a memorable travel experience.</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Nói về một trải nghiệm du lịch đáng nhớ.</v>
-      </c>
-      <c r="C6" t="str">
-        <v>Medium</v>
-      </c>
-      <c r="D6" t="str">
-        <v>2-3 minutes</v>
+        <v>medium</v>
+      </c>
+      <c r="D2">
+        <v>20</v>
+      </c>
+      <c r="E2" t="str">
+        <v>speaking</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>part_number</v>
+      </c>
+      <c r="B1" t="str">
+        <v>title</v>
+      </c>
+      <c r="C1" t="str">
+        <v>description</v>
+      </c>
+      <c r="D1" t="str">
+        <v>instruction</v>
+      </c>
+      <c r="E1" t="str">
+        <v>difficulty_level</v>
+      </c>
+      <c r="F1" t="str">
+        <v>time_limit</v>
+      </c>
+      <c r="G1" t="str">
+        <v>type</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Part 1 - Personal Introduction</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Giới thiệu bản thân và trả lời câu hỏi cá nhân</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Answer the questions about yourself and your background</v>
+      </c>
+      <c r="E2" t="str">
+        <v>medium</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2" t="str">
+        <v>reading</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Part 2 - Describe &amp; Express</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Mô tả hình ảnh và diễn đạt ý kiến</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Describe the picture and express your thoughts</v>
+      </c>
+      <c r="E3" t="str">
+        <v>medium</v>
+      </c>
+      <c r="F3">
+        <v>7</v>
+      </c>
+      <c r="G3" t="str">
+        <v>reading</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Part 3 - Express Opinion</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Trình bày quan điểm về các chủ đề</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Express your opinion on the given topics</v>
+      </c>
+      <c r="E4" t="str">
+        <v>hard</v>
+      </c>
+      <c r="F4">
+        <v>8</v>
+      </c>
+      <c r="G4" t="str">
+        <v>reading</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:G4"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>part_number</v>
+      </c>
+      <c r="B1" t="str">
+        <v>question_number</v>
+      </c>
+      <c r="C1" t="str">
+        <v>content</v>
+      </c>
+      <c r="D1" t="str">
+        <v>question_type</v>
+      </c>
+      <c r="E1" t="str">
+        <v>vietnamese_translation</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Tell me about yourself. What is your name and where are you from?</v>
+      </c>
+      <c r="D2" t="str">
+        <v>essay</v>
+      </c>
+      <c r="E2" t="str">
+        <v>Hãy giới thiệu về bản thân. Tên bạn là gì và bạn đến từ đâu?</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="str">
+        <v>What do you do for work or study? Can you describe your daily routine?</v>
+      </c>
+      <c r="D3" t="str">
+        <v>essay</v>
+      </c>
+      <c r="E3" t="str">
+        <v>Bạn làm công việc gì hoặc học tập như thế nào? Bạn có thể mô tả thói quen hàng ngày của mình không?</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="str">
+        <v>What are your hobbies and interests? Why do you enjoy them?</v>
+      </c>
+      <c r="D4" t="str">
+        <v>essay</v>
+      </c>
+      <c r="E4" t="str">
+        <v>Sở thích và mối quan tâm của bạn là gì? Tại sao bạn thích những điều đó?</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Describe this picture in detail. What do you see and what is happening?</v>
+      </c>
+      <c r="D5" t="str">
+        <v>essay</v>
+      </c>
+      <c r="E5" t="str">
+        <v>Mô tả chi tiết bức tranh này. Bạn nhìn thấy gì và chuyện gì đang xảy ra?</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="str">
+        <v>How does this picture make you feel? What memories or thoughts does it bring?</v>
+      </c>
+      <c r="D6" t="str">
+        <v>essay</v>
+      </c>
+      <c r="E6" t="str">
+        <v>Bức tranh này khiến bạn cảm thấy như thế nào? Nó gợi lên những kỷ niệm hay suy nghĩ gì?</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="str">
+        <v>If you were in this situation, what would you do? Explain your choice.</v>
+      </c>
+      <c r="D7" t="str">
+        <v>essay</v>
+      </c>
+      <c r="E7" t="str">
+        <v>Nếu bạn ở trong tình huống này, bạn sẽ làm gì? Giải thích lựa chọn của bạn.</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Do you think technology has more positive or negative effects on communication? Explain your view.</v>
+      </c>
+      <c r="D8" t="str">
+        <v>essay</v>
+      </c>
+      <c r="E8" t="str">
+        <v>Bạn có nghĩ rằng công nghệ có tác động tích cực hay tiêu cực hơn đến giao tiếp? Giải thích quan điểm của bạn.</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="str">
+        <v>What is the most important quality in a good friend? Give reasons and examples.</v>
+      </c>
+      <c r="D9" t="str">
+        <v>essay</v>
+      </c>
+      <c r="E9" t="str">
+        <v>Đặc điểm quan trọng nhất của một người bạn tốt là gì? Đưa ra lý do và ví dụ.</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Should students be required to learn a foreign language? Why or why not?</v>
+      </c>
+      <c r="D10" t="str">
+        <v>essay</v>
+      </c>
+      <c r="E10" t="str">
+        <v>Có nên bắt buộc học sinh học ngoại ngữ không? Tại sao có hoặc tại sao không?</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="str">
+        <v>How do you think cities will change in the next 20 years? What improvements would you like to see?</v>
+      </c>
+      <c r="D11" t="str">
+        <v>essay</v>
+      </c>
+      <c r="E11" t="str">
+        <v>Bạn nghĩ các thành phố sẽ thay đổi như thế nào trong 20 năm tới? Bạn muốn thấy những cải tiến nào?</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="str">
+        <v>What advice would you give to someone who wants to improve their English speaking skills?</v>
+      </c>
+      <c r="D12" t="str">
+        <v>essay</v>
+      </c>
+      <c r="E12" t="str">
+        <v>Bạn sẽ khuyên gì cho ai đó muốn cải thiện kỹ năng nói tiếng Anh của mình?</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:E12"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>question_number</v>
+      </c>
+      <c r="B1" t="str">
+        <v>content</v>
+      </c>
+      <c r="C1" t="str">
+        <v>is_correct</v>
+      </c>
+      <c r="D1" t="str">
+        <v>explanation</v>
+      </c>
+      <c r="E1" t="str">
+        <v>vietnamese_translation</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v/>
+      </c>
+      <c r="B2" t="str">
+        <v>(Không có đáp án chuẩn cho Speaking Test - đánh giá dựa trên tiêu chí)</v>
+      </c>
+      <c r="C2" t="str">
+        <v/>
+      </c>
+      <c r="D2" t="str">
+        <v/>
+      </c>
+      <c r="E2" t="str">
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
sửa lỗi nhỏ import writing và speaking test
</commit_message>
<xml_diff>
--- a/speaking-test.xlsx
+++ b/speaking-test.xlsx
@@ -1,44 +1,200 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trhuy\Documents\Edutic\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03DE277A-ECC3-47F0-8416-C04BA9311EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Exams" sheetId="1" r:id="rId1"/>
     <sheet name="Parts" sheetId="2" r:id="rId2"/>
     <sheet name="Questions" sheetId="3" r:id="rId3"/>
     <sheet name="Answers" sheetId="4" r:id="rId4"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>difficulty</t>
+  </si>
+  <si>
+    <t>estimated_time</t>
+  </si>
+  <si>
+    <t>exam_type</t>
+  </si>
+  <si>
+    <t>Speaking Test - Assessment</t>
+  </si>
+  <si>
+    <t>Đề thi Speaking - 11 câu hỏi theo chuẩn đánh giá năng lực nói</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>speaking</t>
+  </si>
+  <si>
+    <t>part_number</t>
+  </si>
+  <si>
+    <t>instruction</t>
+  </si>
+  <si>
+    <t>difficulty_level</t>
+  </si>
+  <si>
+    <t>time_limit</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>Part 1 - Personal Introduction</t>
+  </si>
+  <si>
+    <t>Giới thiệu bản thân và trả lời câu hỏi cá nhân</t>
+  </si>
+  <si>
+    <t>Answer the questions about yourself and your background</t>
+  </si>
+  <si>
+    <t>reading</t>
+  </si>
+  <si>
+    <t>Part 2 - Describe &amp; Express</t>
+  </si>
+  <si>
+    <t>Mô tả hình ảnh và diễn đạt ý kiến</t>
+  </si>
+  <si>
+    <t>Describe the picture and express your thoughts</t>
+  </si>
+  <si>
+    <t>Part 3 - Express Opinion</t>
+  </si>
+  <si>
+    <t>Trình bày quan điểm về các chủ đề</t>
+  </si>
+  <si>
+    <t>Express your opinion on the given topics</t>
+  </si>
+  <si>
+    <t>hard</t>
+  </si>
+  <si>
+    <t>question_number</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>question_type</t>
+  </si>
+  <si>
+    <t>vietnamese_translation</t>
+  </si>
+  <si>
+    <t>Tell me about yourself. What is your name and where are you from?</t>
+  </si>
+  <si>
+    <t>Hãy giới thiệu về bản thân. Tên bạn là gì và bạn đến từ đâu?</t>
+  </si>
+  <si>
+    <t>What do you do for work or study? Can you describe your daily routine?</t>
+  </si>
+  <si>
+    <t>Bạn làm công việc gì hoặc học tập như thế nào? Bạn có thể mô tả thói quen hàng ngày của mình không?</t>
+  </si>
+  <si>
+    <t>What are your hobbies and interests? Why do you enjoy them?</t>
+  </si>
+  <si>
+    <t>Sở thích và mối quan tâm của bạn là gì? Tại sao bạn thích những điều đó?</t>
+  </si>
+  <si>
+    <t>Describe this picture in detail. What do you see and what is happening?</t>
+  </si>
+  <si>
+    <t>Mô tả chi tiết bức tranh này. Bạn nhìn thấy gì và chuyện gì đang xảy ra?</t>
+  </si>
+  <si>
+    <t>How does this picture make you feel? What memories or thoughts does it bring?</t>
+  </si>
+  <si>
+    <t>Bức tranh này khiến bạn cảm thấy như thế nào? Nó gợi lên những kỷ niệm hay suy nghĩ gì?</t>
+  </si>
+  <si>
+    <t>If you were in this situation, what would you do? Explain your choice.</t>
+  </si>
+  <si>
+    <t>Nếu bạn ở trong tình huống này, bạn sẽ làm gì? Giải thích lựa chọn của bạn.</t>
+  </si>
+  <si>
+    <t>Do you think technology has more positive or negative effects on communication? Explain your view.</t>
+  </si>
+  <si>
+    <t>Bạn có nghĩ rằng công nghệ có tác động tích cực hay tiêu cực hơn đến giao tiếp? Giải thích quan điểm của bạn.</t>
+  </si>
+  <si>
+    <t>What is the most important quality in a good friend? Give reasons and examples.</t>
+  </si>
+  <si>
+    <t>Đặc điểm quan trọng nhất của một người bạn tốt là gì? Đưa ra lý do và ví dụ.</t>
+  </si>
+  <si>
+    <t>Should students be required to learn a foreign language? Why or why not?</t>
+  </si>
+  <si>
+    <t>Có nên bắt buộc học sinh học ngoại ngữ không? Tại sao có hoặc tại sao không?</t>
+  </si>
+  <si>
+    <t>How do you think cities will change in the next 20 years? What improvements would you like to see?</t>
+  </si>
+  <si>
+    <t>Bạn nghĩ các thành phố sẽ thay đổi như thế nào trong 20 năm tới? Bạn muốn thấy những cải tiến nào?</t>
+  </si>
+  <si>
+    <t>What advice would you give to someone who wants to improve their English speaking skills?</t>
+  </si>
+  <si>
+    <t>Bạn sẽ khuyên gì cho ai đó muốn cải thiện kỹ năng nói tiếng Anh của mình?</t>
+  </si>
+  <si>
+    <t>is_correct</t>
+  </si>
+  <si>
+    <t>explanation</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>(Không có đáp án chuẩn cho Speaking Test - đánh giá dựa trên tiêu chí)</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -75,6 +231,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -399,421 +563,435 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>title</v>
-      </c>
-      <c r="B1" t="str">
-        <v>description</v>
-      </c>
-      <c r="C1" t="str">
-        <v>difficulty</v>
-      </c>
-      <c r="D1" t="str">
-        <v>estimated_time</v>
-      </c>
-      <c r="E1" t="str">
-        <v>exam_type</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Speaking Test - Assessment</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Đề thi Speaking - 11 câu hỏi theo chuẩn đánh giá năng lực nói</v>
-      </c>
-      <c r="C2" t="str">
-        <v>medium</v>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
       </c>
       <c r="D2">
         <v>20</v>
       </c>
-      <c r="E2" t="str">
-        <v>speaking</v>
+      <c r="E2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
+    <ignoredError sqref="A1:E2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>part_number</v>
-      </c>
-      <c r="B1" t="str">
-        <v>title</v>
-      </c>
-      <c r="C1" t="str">
-        <v>description</v>
-      </c>
-      <c r="D1" t="str">
-        <v>instruction</v>
-      </c>
-      <c r="E1" t="str">
-        <v>difficulty_level</v>
-      </c>
-      <c r="F1" t="str">
-        <v>time_limit</v>
-      </c>
-      <c r="G1" t="str">
-        <v>type</v>
-      </c>
-    </row>
-    <row r="2">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="str">
-        <v>Part 1 - Personal Introduction</v>
-      </c>
-      <c r="C2" t="str">
-        <v>Giới thiệu bản thân và trả lời câu hỏi cá nhân</v>
-      </c>
-      <c r="D2" t="str">
-        <v>Answer the questions about yourself and your background</v>
-      </c>
-      <c r="E2" t="str">
-        <v>medium</v>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
       </c>
       <c r="F2">
         <v>5</v>
       </c>
-      <c r="G2" t="str">
-        <v>reading</v>
-      </c>
-    </row>
-    <row r="3">
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="str">
-        <v>Part 2 - Describe &amp; Express</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Mô tả hình ảnh và diễn đạt ý kiến</v>
-      </c>
-      <c r="D3" t="str">
-        <v>Describe the picture and express your thoughts</v>
-      </c>
-      <c r="E3" t="str">
-        <v>medium</v>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
       </c>
       <c r="F3">
         <v>7</v>
       </c>
-      <c r="G3" t="str">
-        <v>reading</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="str">
-        <v>Part 3 - Express Opinion</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Trình bày quan điểm về các chủ đề</v>
-      </c>
-      <c r="D4" t="str">
-        <v>Express your opinion on the given topics</v>
-      </c>
-      <c r="E4" t="str">
-        <v>hard</v>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
       </c>
       <c r="F4">
         <v>8</v>
       </c>
-      <c r="G4" t="str">
-        <v>reading</v>
+      <c r="G4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G4"/>
+    <ignoredError sqref="A1:G4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="32.5" customWidth="1"/>
+    <col min="4" max="4" width="28.75" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>part_number</v>
-      </c>
-      <c r="B1" t="str">
-        <v>question_number</v>
-      </c>
-      <c r="C1" t="str">
-        <v>content</v>
-      </c>
-      <c r="D1" t="str">
-        <v>question_type</v>
-      </c>
-      <c r="E1" t="str">
-        <v>vietnamese_translation</v>
-      </c>
-    </row>
-    <row r="2">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" t="str">
-        <v>Tell me about yourself. What is your name and where are you from?</v>
-      </c>
-      <c r="D2" t="str">
-        <v>essay</v>
-      </c>
-      <c r="E2" t="str">
-        <v>Hãy giới thiệu về bản thân. Tên bạn là gì và bạn đến từ đâu?</v>
-      </c>
-    </row>
-    <row r="3">
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" t="str">
-        <v>What do you do for work or study? Can you describe your daily routine?</v>
-      </c>
-      <c r="D3" t="str">
-        <v>essay</v>
-      </c>
-      <c r="E3" t="str">
-        <v>Bạn làm công việc gì hoặc học tập như thế nào? Bạn có thể mô tả thói quen hàng ngày của mình không?</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" t="str">
-        <v>What are your hobbies and interests? Why do you enjoy them?</v>
-      </c>
-      <c r="D4" t="str">
-        <v>essay</v>
-      </c>
-      <c r="E4" t="str">
-        <v>Sở thích và mối quan tâm của bạn là gì? Tại sao bạn thích những điều đó?</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5" t="str">
-        <v>Describe this picture in detail. What do you see and what is happening?</v>
-      </c>
-      <c r="D5" t="str">
-        <v>essay</v>
-      </c>
-      <c r="E5" t="str">
-        <v>Mô tả chi tiết bức tranh này. Bạn nhìn thấy gì và chuyện gì đang xảy ra?</v>
-      </c>
-    </row>
-    <row r="6">
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
-      <c r="C6" t="str">
-        <v>How does this picture make you feel? What memories or thoughts does it bring?</v>
-      </c>
-      <c r="D6" t="str">
-        <v>essay</v>
-      </c>
-      <c r="E6" t="str">
-        <v>Bức tranh này khiến bạn cảm thấy như thế nào? Nó gợi lên những kỷ niệm hay suy nghĩ gì?</v>
-      </c>
-    </row>
-    <row r="7">
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
-      <c r="C7" t="str">
-        <v>If you were in this situation, what would you do? Explain your choice.</v>
-      </c>
-      <c r="D7" t="str">
-        <v>essay</v>
-      </c>
-      <c r="E7" t="str">
-        <v>Nếu bạn ở trong tình huống này, bạn sẽ làm gì? Giải thích lựa chọn của bạn.</v>
-      </c>
-    </row>
-    <row r="8">
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
-      <c r="C8" t="str">
-        <v>Do you think technology has more positive or negative effects on communication? Explain your view.</v>
-      </c>
-      <c r="D8" t="str">
-        <v>essay</v>
-      </c>
-      <c r="E8" t="str">
-        <v>Bạn có nghĩ rằng công nghệ có tác động tích cực hay tiêu cực hơn đến giao tiếp? Giải thích quan điểm của bạn.</v>
-      </c>
-    </row>
-    <row r="9">
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
-      <c r="C9" t="str">
-        <v>What is the most important quality in a good friend? Give reasons and examples.</v>
-      </c>
-      <c r="D9" t="str">
-        <v>essay</v>
-      </c>
-      <c r="E9" t="str">
-        <v>Đặc điểm quan trọng nhất của một người bạn tốt là gì? Đưa ra lý do và ví dụ.</v>
-      </c>
-    </row>
-    <row r="10">
+      <c r="C9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
-      <c r="C10" t="str">
-        <v>Should students be required to learn a foreign language? Why or why not?</v>
-      </c>
-      <c r="D10" t="str">
-        <v>essay</v>
-      </c>
-      <c r="E10" t="str">
-        <v>Có nên bắt buộc học sinh học ngoại ngữ không? Tại sao có hoặc tại sao không?</v>
-      </c>
-    </row>
-    <row r="11">
+      <c r="C10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
-      <c r="C11" t="str">
-        <v>How do you think cities will change in the next 20 years? What improvements would you like to see?</v>
-      </c>
-      <c r="D11" t="str">
-        <v>essay</v>
-      </c>
-      <c r="E11" t="str">
-        <v>Bạn nghĩ các thành phố sẽ thay đổi như thế nào trong 20 năm tới? Bạn muốn thấy những cải tiến nào?</v>
-      </c>
-    </row>
-    <row r="12">
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
       <c r="B12">
         <v>11</v>
       </c>
-      <c r="C12" t="str">
-        <v>What advice would you give to someone who wants to improve their English speaking skills?</v>
-      </c>
-      <c r="D12" t="str">
-        <v>essay</v>
-      </c>
-      <c r="E12" t="str">
-        <v>Bạn sẽ khuyên gì cho ai đó muốn cải thiện kỹ năng nói tiếng Anh của mình?</v>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E12"/>
+    <ignoredError sqref="A1:E1 A5:C12 A2:C2 E2 A3:C3 E3 A4:C4 E4 E5:E12" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>question_number</v>
-      </c>
-      <c r="B1" t="str">
-        <v>content</v>
-      </c>
-      <c r="C1" t="str">
-        <v>is_correct</v>
-      </c>
-      <c r="D1" t="str">
-        <v>explanation</v>
-      </c>
-      <c r="E1" t="str">
-        <v>vietnamese_translation</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v/>
-      </c>
-      <c r="B2" t="str">
-        <v>(Không có đáp án chuẩn cho Speaking Test - đánh giá dựa trên tiêu chí)</v>
-      </c>
-      <c r="C2" t="str">
-        <v/>
-      </c>
-      <c r="D2" t="str">
-        <v/>
-      </c>
-      <c r="E2" t="str">
-        <v/>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
+    <ignoredError sqref="A1:E2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>